<commit_message>
# Feature 4 File management load/unload script
</commit_message>
<xml_diff>
--- a/SavedFile/test.xlsx
+++ b/SavedFile/test.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>MacroActionType</t>
   </si>
@@ -35,7 +35,7 @@
     <t>Left</t>
   </si>
   <si>
-    <t>373, 231</t>
+    <t>134, 124</t>
   </si>
   <si>
     <t>1</t>
@@ -47,22 +47,16 @@
     <t>KeyPress</t>
   </si>
   <si>
-    <t>Key Press: 'K'</t>
-  </si>
-  <si>
-    <t>K</t>
-  </si>
-  <si>
-    <t>Key Press: 'r'</t>
-  </si>
-  <si>
-    <t>r</t>
-  </si>
-  <si>
-    <t>Key Press: 'i'</t>
-  </si>
-  <si>
-    <t>i</t>
+    <t>Key Press: 't'</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>Key Press: 'e'</t>
+  </si>
+  <si>
+    <t>e</t>
   </si>
   <si>
     <t>Key Press: 's'</t>
@@ -71,28 +65,10 @@
     <t>s</t>
   </si>
   <si>
-    <t>Key Press: 't'</t>
-  </si>
-  <si>
-    <t>t</t>
-  </si>
-  <si>
-    <t>Key Press: 'a'</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>Key Press: 'n'</t>
-  </si>
-  <si>
-    <t>n</t>
-  </si>
-  <si>
-    <t>1102, 1076</t>
-  </si>
-  <si>
-    <t>1821, 216</t>
+    <t>618, 759</t>
+  </si>
+  <si>
+    <t>1275, 165</t>
   </si>
 </sst>
 </file>
@@ -138,7 +114,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -234,13 +210,13 @@
         <v>10</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E6" s="0" t="s">
         <v>9</v>
@@ -248,16 +224,16 @@
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E7" s="0" t="s">
         <v>9</v>
@@ -265,86 +241,18 @@
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="0" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>